<commit_message>
Analysis primary quench (unfinished)
</commit_message>
<xml_diff>
--- a/data/20220707_acquisition_summary.xlsx
+++ b/data/20220707_acquisition_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\SWAN_projects\lhc-anomaly-detection\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7CE115-1750-4F37-B524-6E149A1864E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D82D776-1C27-45E2-9E56-1014AE0DB39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3152,8 +3152,8 @@
   <dimension ref="A1:O897"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A840" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F858" sqref="F858"/>
+      <pane ySplit="1" topLeftCell="A465" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F485" sqref="F485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3747,10 +3747,10 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -4247,7 +4247,7 @@
         <v>1</v>
       </c>
       <c r="O23">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -25555,10 +25555,10 @@
         <v>1</v>
       </c>
       <c r="E477">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F477">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G477">
         <v>1</v>
@@ -25585,7 +25585,7 @@
         <v>1</v>
       </c>
       <c r="O477">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="478" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>